<commit_message>
Logbook is now configurable and text is aligned
</commit_message>
<xml_diff>
--- a/MP3 Creation/speech.xlsx
+++ b/MP3 Creation/speech.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="617" yWindow="69" windowWidth="31749" windowHeight="15240"/>
+    <workbookView xWindow="617" yWindow="69" windowWidth="31749" windowHeight="15240" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ivy" sheetId="1" r:id="rId1"/>
@@ -1483,21 +1483,6 @@
     <t>Audacity</t>
   </si>
   <si>
-    <t>Verzerren</t>
-  </si>
-  <si>
-    <t>Sanftes Abschneiden</t>
-  </si>
-  <si>
-    <t>Schwelle -18</t>
-  </si>
-  <si>
-    <t>Härtegrad 51</t>
-  </si>
-  <si>
-    <t>Makeup Gain 29</t>
-  </si>
-  <si>
     <t>&lt;speak&gt;
 &lt;emphasis level="moderate"&gt; Dear &lt;/emphasis&gt; passengers  , we are now ready for &lt;emphasis level="moderate"&gt;departure&lt;/emphasis&gt;. 
 Please put your seats into an upright position,
@@ -1580,6 +1565,25 @@
   </si>
   <si>
     <t>landing</t>
+  </si>
+  <si>
+    <t>minimums</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+approaching minimums
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+Positive rate
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>Low Pass Filter: f=1000Hz, 6db</t>
+  </si>
+  <si>
+    <t>Amplify: Ratio=1.303</t>
   </si>
 </sst>
 </file>
@@ -1923,8 +1927,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -1994,7 +1999,9 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -2646,7 +2653,7 @@
         <v>102</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>273</v>
@@ -3095,10 +3102,10 @@
         <v>226</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>227</v>
@@ -3116,10 +3123,10 @@
         <v>231</v>
       </c>
       <c r="K70" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="L70" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
@@ -3128,7 +3135,7 @@
     </row>
     <row r="71" spans="1:16" ht="276.89999999999998">
       <c r="A71" s="3" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>232</v>
@@ -3152,7 +3159,7 @@
         <v>238</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="J71" s="2" t="s">
         <v>239</v>
@@ -3170,7 +3177,7 @@
         <v>242</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>243</v>
@@ -3194,9 +3201,13 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
-      <c r="A73" s="3"/>
-      <c r="B73" s="2"/>
+    <row r="73" spans="1:16" ht="43.75">
+      <c r="A73" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -9024,10 +9035,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -9048,27 +9059,12 @@
         <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slats bug fixed Exchanged two mp3s (used explicit gender)
</commit_message>
<xml_diff>
--- a/MP3 Creation/speech.xlsx
+++ b/MP3 Creation/speech.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="617" yWindow="69" windowWidth="31749" windowHeight="15240" activeTab="3"/>
+    <workbookView xWindow="617" yWindow="69" windowWidth="31749" windowHeight="15240"/>
   </bookViews>
   <sheets>
     <sheet name="Ivy" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="295">
   <si>
     <t>EVENT</t>
   </si>
@@ -328,16 +328,6 @@
   </si>
   <si>
     <t>cabin_down_fast</t>
-  </si>
-  <si>
-    <t>&lt;speak&gt;
-&lt;prosody pitch="high" rate ="fast"&gt;
-I think my ears are popping! It hurts so
-&lt;/prosody&gt; 
-&lt;prosody pitch="x-high" rate ="medium"&gt;
-much!
-&lt;/prosody&gt;
-&lt;/speak&gt;</t>
   </si>
   <si>
     <t>&lt;speak&gt;
@@ -1187,18 +1177,6 @@
   <si>
     <t>&lt;speak&gt;
 Dear passengers, we are about to land.
-Our  captain is &lt;emphasis level="moderate"&gt; well prepared.&lt;/emphasis&gt;
-&lt;emphasis level="strong"&gt;No&lt;/emphasis&gt; wind shear,
-&lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; microburst,
-&lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; lightning strike,
-and &lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; engine explosion, will keep him from landing safely. 
-&lt;prosody rate ="fast"&gt;  &lt;emphasis level="reduced"&gt; At least, this is what he tries to convince himself.&lt;/emphasis&gt;&lt;/prosody&gt;
-We hope you enjoyed the flight and wish you a pleasant stay.
-&lt;/speak&gt;</t>
-  </si>
-  <si>
-    <t>&lt;speak&gt;
-Dear passengers, we are about to land.
 This is an absolutely safe procedure, and there is nothing to worry about.
 &lt;emphasis level="reduced"&gt;
 Except, if we hit the ground with the wingtip first.
@@ -1584,6 +1562,35 @@
   </si>
   <si>
     <t>Amplify: Ratio=1.303</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+&lt;prosody pitch="high" rate ="fast"&gt;
+I think my ears are popping! &lt;/prosody&gt; 
+&lt;prosody pitch="x-high" rate ="medium"&gt;
+&lt;/prosody&gt;
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+&lt;emphasis level="moderate"&gt; Dear &lt;/emphasis&gt; passengers  , we are now ready for &lt;emphasis level="moderate"&gt;take off&lt;/emphasis&gt;. 
+Would you &lt;emphasis level="moderate"&gt; please &lt;/emphasis&gt; fasten your seat-belts &lt;emphasis level="moderate"&gt; as tight as possible &lt;/emphasis&gt; and switch off your mobile phones.
+Our captain will bring you safely into the air. 
+There is no need to fear bird strikes, engine fires, lightning strikes, or deer crashing into our aircraft, 
+as our captain is well prepared for &lt;emphasis level="moderate"&gt; all &lt;/emphasis&gt; situations.
+We wish you a &lt;emphasis level="moderate"&gt; pleasant  flight.&lt;/emphasis&gt;
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+Dear passengers, we are about to land.
+Our  captain is &lt;emphasis level="moderate"&gt; well prepared.&lt;/emphasis&gt;
+&lt;emphasis level="strong"&gt;No&lt;/emphasis&gt; wind shear,
+&lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; microburst,
+&lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; lightning strike,
+and &lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; engine explosion, will keep our captain from landing safely. 
+We hope you enjoyed the flight and wish you a pleasant stay.
+&lt;/speak&gt;</t>
   </si>
 </sst>
 </file>
@@ -1927,9 +1934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P601"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -1985,7 +1992,7 @@
     </row>
     <row r="2" spans="1:11" ht="58.3">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -1994,13 +2001,13 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2010,7 +2017,7 @@
     </row>
     <row r="3" spans="1:11" ht="43.75">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -2027,7 +2034,7 @@
     </row>
     <row r="4" spans="1:11" ht="43.75">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -2044,16 +2051,16 @@
     </row>
     <row r="5" spans="1:11" ht="72.900000000000006">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2065,19 +2072,19 @@
     </row>
     <row r="6" spans="1:11" ht="96" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2088,7 +2095,7 @@
     </row>
     <row r="7" spans="1:11" ht="43.75">
       <c r="A7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
@@ -2105,19 +2112,19 @@
     </row>
     <row r="8" spans="1:11" ht="102">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2128,16 +2135,16 @@
     </row>
     <row r="9" spans="1:11" ht="58.3">
       <c r="A9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2149,7 +2156,7 @@
     </row>
     <row r="10" spans="1:11" ht="87.45">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>20</v>
@@ -2158,7 +2165,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -2170,7 +2177,7 @@
     </row>
     <row r="11" spans="1:11" ht="43.75">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
@@ -2257,7 +2264,7 @@
         <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="72.900000000000006">
@@ -2290,16 +2297,16 @@
         <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="102">
@@ -2310,13 +2317,13 @@
         <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="102">
@@ -2327,10 +2334,10 @@
         <v>51</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -2342,16 +2349,16 @@
         <v>52</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2375,15 +2382,15 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="116.6">
+    <row r="24" spans="1:8" ht="87.45">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2393,13 +2400,13 @@
     </row>
     <row r="25" spans="1:8" ht="43.75">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2409,41 +2416,41 @@
     </row>
     <row r="26" spans="1:8" ht="87.45">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="58.3">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="D27" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2451,13 +2458,13 @@
     </row>
     <row r="28" spans="1:8" ht="43.75">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2467,19 +2474,19 @@
     </row>
     <row r="29" spans="1:8" ht="43.75">
       <c r="A29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2487,10 +2494,10 @@
     </row>
     <row r="30" spans="1:8" ht="43.75">
       <c r="A30" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2501,10 +2508,10 @@
     </row>
     <row r="31" spans="1:8" ht="58.3">
       <c r="A31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2515,10 +2522,10 @@
     </row>
     <row r="32" spans="1:8" ht="43.75">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -2529,13 +2536,13 @@
     </row>
     <row r="33" spans="1:8" ht="43.75">
       <c r="A33" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>209</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2545,19 +2552,19 @@
     </row>
     <row r="34" spans="1:8" ht="58.3">
       <c r="A34" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2565,10 +2572,10 @@
     </row>
     <row r="35" spans="1:8" ht="43.75">
       <c r="A35" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -2579,10 +2586,10 @@
     </row>
     <row r="36" spans="1:8" ht="58.3">
       <c r="A36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2593,10 +2600,10 @@
     </row>
     <row r="37" spans="1:8" ht="335.15">
       <c r="A37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2607,19 +2614,19 @@
     </row>
     <row r="38" spans="1:8" ht="58.3">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -2627,19 +2634,19 @@
     </row>
     <row r="39" spans="1:8" ht="43.75">
       <c r="A39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -2647,19 +2654,19 @@
     </row>
     <row r="40" spans="1:8" ht="72.900000000000006">
       <c r="A40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -2667,16 +2674,16 @@
     </row>
     <row r="41" spans="1:8" ht="87.45">
       <c r="A41" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2685,13 +2692,13 @@
     </row>
     <row r="42" spans="1:8" ht="87.45">
       <c r="A42" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2701,16 +2708,16 @@
     </row>
     <row r="43" spans="1:8" ht="43.75">
       <c r="A43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -2719,10 +2726,10 @@
     </row>
     <row r="44" spans="1:8" ht="43.75">
       <c r="A44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2733,13 +2740,13 @@
     </row>
     <row r="45" spans="1:8" ht="58.3">
       <c r="A45" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2749,13 +2756,13 @@
     </row>
     <row r="46" spans="1:8" ht="58.3">
       <c r="A46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2765,10 +2772,10 @@
     </row>
     <row r="47" spans="1:8" ht="58.3">
       <c r="A47" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2779,10 +2786,10 @@
     </row>
     <row r="48" spans="1:8" ht="43.75">
       <c r="A48" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2793,10 +2800,10 @@
     </row>
     <row r="49" spans="1:8" ht="43.75">
       <c r="A49" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2807,10 +2814,10 @@
     </row>
     <row r="50" spans="1:8" ht="43.75">
       <c r="A50" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2821,10 +2828,10 @@
     </row>
     <row r="51" spans="1:8" ht="43.75">
       <c r="A51" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2835,10 +2842,10 @@
     </row>
     <row r="52" spans="1:8" ht="43.75">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2849,10 +2856,10 @@
     </row>
     <row r="53" spans="1:8" ht="43.75">
       <c r="A53" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2863,10 +2870,10 @@
     </row>
     <row r="54" spans="1:8" ht="43.75">
       <c r="A54" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2877,10 +2884,10 @@
     </row>
     <row r="55" spans="1:8" ht="58.3">
       <c r="A55" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2891,10 +2898,10 @@
     </row>
     <row r="56" spans="1:8" ht="43.75">
       <c r="A56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2905,10 +2912,10 @@
     </row>
     <row r="57" spans="1:8" ht="43.75">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2919,10 +2926,10 @@
     </row>
     <row r="58" spans="1:8" ht="43.75">
       <c r="A58" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2933,10 +2940,10 @@
     </row>
     <row r="59" spans="1:8" ht="43.75">
       <c r="A59" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2947,10 +2954,10 @@
     </row>
     <row r="60" spans="1:8" ht="43.75">
       <c r="A60" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2961,10 +2968,10 @@
     </row>
     <row r="61" spans="1:8" ht="43.75">
       <c r="A61" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2975,10 +2982,10 @@
     </row>
     <row r="62" spans="1:8" ht="43.75">
       <c r="A62" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2989,10 +2996,10 @@
     </row>
     <row r="63" spans="1:8" ht="43.75">
       <c r="A63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>169</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3003,19 +3010,19 @@
     </row>
     <row r="64" spans="1:8" ht="174.9">
       <c r="A64" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -3023,10 +3030,10 @@
     </row>
     <row r="65" spans="1:16" ht="43.75">
       <c r="A65" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3037,10 +3044,10 @@
     </row>
     <row r="66" spans="1:16" ht="43.75">
       <c r="A66" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -3051,10 +3058,10 @@
     </row>
     <row r="67" spans="1:16" ht="43.75">
       <c r="A67" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3065,10 +3072,10 @@
     </row>
     <row r="68" spans="1:16" ht="43.75">
       <c r="A68" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3079,10 +3086,10 @@
     </row>
     <row r="69" spans="1:16" ht="43.75">
       <c r="A69" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3093,40 +3100,40 @@
     </row>
     <row r="70" spans="1:16" ht="189.45">
       <c r="A70" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="D70" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="H70" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="J70" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="J70" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="K70" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L70" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
@@ -3135,78 +3142,78 @@
     </row>
     <row r="71" spans="1:16" ht="276.89999999999998">
       <c r="A71" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="H71" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J71" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="K71" s="2"/>
     </row>
     <row r="72" spans="1:16" ht="276.89999999999998">
       <c r="A72" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="D72" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="F72" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="K72" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="J72" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="43.75">
       <c r="A73" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
@@ -8520,57 +8527,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -8640,227 +8647,227 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -8886,146 +8893,146 @@
   <sheetData>
     <row r="1" spans="1:2" ht="43.75">
       <c r="A1" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="43.75">
       <c r="A2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.75">
       <c r="A3" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="43.75">
       <c r="A4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="43.75">
       <c r="A5" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.75">
       <c r="A6" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.75">
       <c r="A7" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.75">
       <c r="A8" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>173</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="43.75">
       <c r="A9" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="43.75">
       <c r="A10" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="43.75">
       <c r="A11" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="43.75">
       <c r="A12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="43.75">
       <c r="A14" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="43.75">
       <c r="A15" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="43.75">
       <c r="A16" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.75">
       <c r="A17" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="131.15">
       <c r="A18" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -9037,7 +9044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9048,23 +9055,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added custom v-speeds when no dataref is present Added decision height to v-speed dialog Added settings for 60, 80, and 100 kt call out
</commit_message>
<xml_diff>
--- a/MP3 Creation/speech.xlsx
+++ b/MP3 Creation/speech.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="299">
   <si>
     <t>EVENT</t>
   </si>
@@ -1590,6 +1590,22 @@
 &lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; lightning strike,
 and &lt;emphasis level="strong"&gt;no&lt;/emphasis&gt; engine explosion, will keep our captain from landing safely. 
 We hope you enjoyed the flight and wish you a pleasant stay.
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>80kt</t>
+  </si>
+  <si>
+    <t>100kt</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+80 knots
+&lt;/speak&gt;</t>
+  </si>
+  <si>
+    <t>&lt;speak&gt;
+100 knots
 &lt;/speak&gt;</t>
   </si>
 </sst>
@@ -1932,11 +1948,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P601"/>
+  <dimension ref="A1:P603"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>
@@ -2726,10 +2742,10 @@
     </row>
     <row r="44" spans="1:8" ht="43.75">
       <c r="A44" s="3" t="s">
-        <v>116</v>
+        <v>295</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>117</v>
+        <v>297</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2738,32 +2754,28 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" ht="58.3">
+    <row r="45" spans="1:8" ht="43.75">
       <c r="A45" s="3" t="s">
-        <v>118</v>
+        <v>296</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>119</v>
-      </c>
+        <v>298</v>
+      </c>
+      <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="58.3">
+    <row r="46" spans="1:8" ht="43.75">
       <c r="A46" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>122</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2772,38 +2784,42 @@
     </row>
     <row r="47" spans="1:8" ht="58.3">
       <c r="A47" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="2"/>
+        <v>149</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="43.75">
+    <row r="48" spans="1:8" ht="58.3">
       <c r="A48" s="3" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>121</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="43.75">
+    <row r="49" spans="1:8" ht="58.3">
       <c r="A49" s="3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2814,10 +2830,10 @@
     </row>
     <row r="50" spans="1:8" ht="43.75">
       <c r="A50" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2828,10 +2844,10 @@
     </row>
     <row r="51" spans="1:8" ht="43.75">
       <c r="A51" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2842,10 +2858,10 @@
     </row>
     <row r="52" spans="1:8" ht="43.75">
       <c r="A52" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2856,10 +2872,10 @@
     </row>
     <row r="53" spans="1:8" ht="43.75">
       <c r="A53" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2870,10 +2886,10 @@
     </row>
     <row r="54" spans="1:8" ht="43.75">
       <c r="A54" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2882,12 +2898,12 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="58.3">
+    <row r="55" spans="1:8" ht="43.75">
       <c r="A55" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2898,10 +2914,10 @@
     </row>
     <row r="56" spans="1:8" ht="43.75">
       <c r="A56" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2910,12 +2926,12 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" ht="43.75">
+    <row r="57" spans="1:8" ht="58.3">
       <c r="A57" s="3" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2926,10 +2942,10 @@
     </row>
     <row r="58" spans="1:8" ht="43.75">
       <c r="A58" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2940,10 +2956,10 @@
     </row>
     <row r="59" spans="1:8" ht="43.75">
       <c r="A59" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2954,10 +2970,10 @@
     </row>
     <row r="60" spans="1:8" ht="43.75">
       <c r="A60" s="3" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2968,10 +2984,10 @@
     </row>
     <row r="61" spans="1:8" ht="43.75">
       <c r="A61" s="3" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2982,10 +2998,10 @@
     </row>
     <row r="62" spans="1:8" ht="43.75">
       <c r="A62" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2996,10 +3012,10 @@
     </row>
     <row r="63" spans="1:8" ht="43.75">
       <c r="A63" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -3008,32 +3024,26 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="174.9">
+    <row r="64" spans="1:8" ht="43.75">
       <c r="A64" s="3" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>274</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:16" ht="43.75">
       <c r="A65" s="3" t="s">
-        <v>197</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -3042,26 +3052,32 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:16" ht="43.75">
-      <c r="A66" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+    <row r="66" spans="1:16" ht="174.9">
+      <c r="A66" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>274</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:16" ht="43.75">
-      <c r="A67" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>180</v>
+      <c r="A67" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -3071,11 +3087,11 @@
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:16" ht="43.75">
-      <c r="A68" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>185</v>
+      <c r="A68" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -3085,11 +3101,11 @@
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:16" ht="43.75">
-      <c r="A69" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>184</v>
+      <c r="A69" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -3098,146 +3114,154 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:16" ht="189.45">
+    <row r="70" spans="1:16" ht="43.75">
       <c r="A70" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:16" ht="43.75">
+      <c r="A71" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:16" ht="189.45">
+      <c r="A72" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="E72" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G70" s="2" t="s">
+      <c r="G72" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="H72" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="J70" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K70" s="2" t="s">
+      <c r="K72" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3"/>
-      <c r="P70" s="3"/>
-    </row>
-    <row r="71" spans="1:16" ht="276.89999999999998">
-      <c r="A71" s="3" t="s">
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
+      <c r="P72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" ht="276.89999999999998">
+      <c r="A73" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E73" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F73" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="G73" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="H73" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="J73" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="K71" s="2"/>
-    </row>
-    <row r="72" spans="1:16" ht="276.89999999999998">
-      <c r="A72" s="3" t="s">
+      <c r="K73" s="2"/>
+    </row>
+    <row r="74" spans="1:16" ht="276.89999999999998">
+      <c r="A74" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G72" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="H74" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="I72" s="1" t="s">
+      <c r="I74" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="J72" s="1" t="s">
+      <c r="J74" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="K74" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="43.75">
-      <c r="A73" s="3" t="s">
+    <row r="75" spans="1:16" ht="43.75">
+      <c r="A75" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="1:16">
-      <c r="A74" s="3"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:16">
-      <c r="A75" s="3"/>
-      <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
@@ -8500,6 +8524,26 @@
       <c r="F601" s="2"/>
       <c r="G601" s="2"/>
       <c r="H601" s="2"/>
+    </row>
+    <row r="602" spans="1:8">
+      <c r="A602" s="3"/>
+      <c r="B602" s="2"/>
+      <c r="C602" s="2"/>
+      <c r="D602" s="2"/>
+      <c r="E602" s="2"/>
+      <c r="F602" s="2"/>
+      <c r="G602" s="2"/>
+      <c r="H602" s="2"/>
+    </row>
+    <row r="603" spans="1:8">
+      <c r="A603" s="3"/>
+      <c r="B603" s="2"/>
+      <c r="C603" s="2"/>
+      <c r="D603" s="2"/>
+      <c r="E603" s="2"/>
+      <c r="F603" s="2"/>
+      <c r="G603" s="2"/>
+      <c r="H603" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Not sure what I changed, but Excel file was updated
</commit_message>
<xml_diff>
--- a/MP3 Creation/speech.xlsx
+++ b/MP3 Creation/speech.xlsx
@@ -1951,8 +1951,8 @@
   <dimension ref="A1:P603"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6"/>

</xml_diff>